<commit_message>
[tsomsomm] : manual full rebuild
</commit_message>
<xml_diff>
--- a/data/_meta/LocalData.xlsx
+++ b/data/_meta/LocalData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,6 +567,48 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ItemData.Item.1000004</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>솔라리</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MapNpcData.MapNpcMenu.1000005.1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>컷신1 재성</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MapNpcData.MapNpcMenu.1000005.2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>컷신2 재생</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[tsomsomm] : add CharacterData
</commit_message>
<xml_diff>
--- a/data/_meta/LocalData.xlsx
+++ b/data/_meta/LocalData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MapNpcData.MapNpcMenu.1000000.1</t>
+          <t>CharacterData.CharacterInfo.1000003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>컷신1 재성</t>
+          <t>테스트용 캐릭터</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -472,16 +472,114 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MapNpcData.MapNpcMenu.1000000.2</t>
+          <t>CutsceneData.Cutscene.1000001.1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>컷신2 재생</t>
+          <t>ShowDialog</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CutsceneData.Cutscene.1000001.2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ShowDialogFlipped</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CutsceneData.Cutscene.1000002.4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ShowDialog</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CutsceneData.Cutscene.1000002.5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ShowDialogFlipped</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CutsceneData.CutsceneInfo.1000001</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>컷신이름1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CutsceneData.CutsceneInfo.1000002</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>컷신이름2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CutsceneData.CutsceneSelection.1000004</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>선택지1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CutsceneData.CutsceneSelection.1000005</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>선택지2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[heewkim112] : Revert 컷씬테스트3
</commit_message>
<xml_diff>
--- a/data/_meta/LocalData.xlsx
+++ b/data/_meta/LocalData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -697,13 +697,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CutsceneData.Cutscene.1000013.10</t>
+          <t>CutsceneData.CutsceneSelection.1000004</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>축하드립니다! 
-이제 어엿한 마법소녀라고 할 수 있겠네요!</t>
+          <t>선택지1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -712,12 +711,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CutsceneData.CutsceneSelection.1000004</t>
+          <t>CutsceneData.CutsceneSelection.1000005</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>선택지1</t>
+          <t>선택지2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -726,12 +725,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CutsceneData.CutsceneSelection.1000005</t>
+          <t>CutsceneData.CutsceneSelection.1000014</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>선택지2</t>
+          <t>맞아</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -740,12 +739,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CutsceneData.CutsceneSelection.1000014</t>
+          <t>CutsceneData.CutsceneSelection.1000015</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>맞아</t>
+          <t>글쎄?</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -754,12 +753,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CutsceneData.CutsceneSelection.1000015</t>
+          <t>ItemData.Item.1000006</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>글쎄?</t>
+          <t>솔라리</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -768,12 +767,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ItemData.Item.1000006</t>
+          <t>ItemData.Item.1000018</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>솔라리</t>
+          <t>스틱</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -782,12 +781,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ItemData.Item.1000018</t>
+          <t>ItemData.Item.1000019</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>스틱</t>
+          <t>파우더</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -796,12 +795,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ItemData.Item.1000019</t>
+          <t>ItemData.Item.1000020</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>파우더</t>
+          <t>버블건</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -810,12 +809,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ItemData.Item.1000020</t>
+          <t>ItemData.Item.1000021</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>버블건</t>
+          <t>그라인더</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -824,12 +823,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ItemData.Item.1000021</t>
+          <t>ItemData.Item.1000022</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>그라인더</t>
+          <t>펜던트</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -838,12 +837,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ItemData.Item.1000022</t>
+          <t>LoadingData.Loading.1000007</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>펜던트</t>
+          <t>로딩 내용 어쩌고 저쩌고1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -852,12 +851,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LoadingData.Loading.1000007</t>
+          <t>LoadingData.Loading.1000008</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>로딩 내용 어쩌고 저쩌고1</t>
+          <t>로딩 내용 어쩌고 저쩌고2</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -866,12 +865,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LoadingData.Loading.1000008</t>
+          <t>MapNpcData.MapNpcMenu.1000000.1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>로딩 내용 어쩌고 저쩌고2</t>
+          <t>컷신1 재성</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -880,12 +879,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MapNpcData.MapNpcMenu.1000000.1</t>
+          <t>MapNpcData.MapNpcMenu.1000000.2</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>컷신1 재성</t>
+          <t>컷신2 재생</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -894,12 +893,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MapNpcData.MapNpcMenu.1000000.2</t>
+          <t>MapNpcData.MapNpcMenu.1000009.1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>컷신2 재생</t>
+          <t>말걸기</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -908,30 +907,16 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MapNpcData.MapNpcMenu.1000009.1</t>
+          <t>MapNpcData.MapNpcMenu.1000009.2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>말걸기</t>
+          <t>미니게임 시작</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>MapNpcData.MapNpcMenu.1000009.2</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>미니게임 시작</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[tsomsomm] : [Npc] 마이홈 npc
</commit_message>
<xml_diff>
--- a/data/_meta/LocalData.xlsx
+++ b/data/_meta/LocalData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1128,6 +1128,20 @@
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>MapNpcData.MapNpcMenu.1000023.1</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>마이홈 돌아가기</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[tsomsomm] : LoadingType 추가
</commit_message>
<xml_diff>
--- a/data/_meta/LocalData.xlsx
+++ b/data/_meta/LocalData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,12 +1103,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MapNpcData.MapNpcMenu.1000009.1</t>
+          <t>LoadingData.Loading.1000027</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>말걸기</t>
+          <t>솜사탕상점 로딩화면</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -1117,16 +1117,58 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MapNpcData.MapNpcMenu.1000009.2</t>
+          <t>LoadingData.Loading.1000028</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>미니게임 시작</t>
+          <t>파우더상점 로딩화면</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>LoadingData.Loading.1000029</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>이불상점 로딩화면</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>MapNpcData.MapNpcMenu.1000009.1</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>말걸기</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>MapNpcData.MapNpcMenu.1000009.2</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>미니게임 시작</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>